<commit_message>
Continued working on getting the formula to place each value in the array correct.
</commit_message>
<xml_diff>
--- a/7 node grid.xlsx
+++ b/7 node grid.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Round 1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="222">
   <si>
     <t>1.2.3</t>
   </si>
@@ -673,9 +673,6 @@
     <t>+sender</t>
   </si>
   <si>
-    <t>+((I+1) / (nG -rn)) * messageSize)</t>
-  </si>
-  <si>
     <t>+ sender - rn</t>
   </si>
   <si>
@@ -689,6 +686,12 @@
   </si>
   <si>
     <t>messageSize:</t>
+  </si>
+  <si>
+    <t>+sender - rn</t>
+  </si>
+  <si>
+    <t>+((I / (nG - rn)) + 1) * messageSize)</t>
   </si>
 </sst>
 </file>
@@ -724,7 +727,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -966,11 +969,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -993,6 +1014,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1273,78 +1296,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B22"/>
+  <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D2" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="20"/>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="20"/>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="20"/>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="19">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="20"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -1382,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,13 +1450,13 @@
         <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="R2">
         <v>6</v>
@@ -1483,12 +1518,24 @@
         <v>2</v>
       </c>
       <c r="M5">
-        <f>$J5*COUNTA($J$5:$J$10)+$K$2-1</f>
+        <f>$J5*$R$2+$K$2-1</f>
         <v>2</v>
       </c>
       <c r="N5">
-        <f>(($J5+1)*6) + $K$2</f>
+        <f>(($J5+1)*$R$2) + $K$2</f>
         <v>9</v>
+      </c>
+      <c r="P5">
+        <f>(J5/$R$2)*6</f>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f>P5*$R$2</f>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f>(P5+1)*$R$2</f>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -1517,12 +1564,24 @@
         <v>8</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M10" si="0">$J6*COUNTA($J$5:$J$10)+$K$2-1</f>
+        <f t="shared" ref="M6:M10" si="0">$J6*$R$2+$K$2-1</f>
         <v>8</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N6:N10" si="1">(($J6+1)*6) + $K$2</f>
+        <f t="shared" ref="N6:N10" si="1">(($J6+1)*$R$2) + $K$2</f>
         <v>15</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P10" si="2">(J6/$R$2)*6</f>
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q10" si="3">P6*$R$2</f>
+        <v>6</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R10" si="4">(P6+1)*$R$2</f>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1548,6 +1607,18 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="12">
@@ -1582,6 +1653,18 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
@@ -1615,6 +1698,18 @@
       <c r="N9">
         <f t="shared" si="1"/>
         <v>33</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="4"/>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1639,6 +1734,18 @@
       <c r="N10">
         <f t="shared" si="1"/>
         <v>39</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="4"/>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
@@ -1689,7 +1796,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="17"/>
       <c r="J13" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L13" s="21" t="s">
         <v>212</v>
@@ -1735,10 +1842,10 @@
         <v>29</v>
       </c>
       <c r="J15" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="L15" s="21" t="s">
         <v>217</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1858,10 +1965,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AE55"/>
+  <dimension ref="B1:AE60"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,44 +2159,44 @@
       </c>
     </row>
     <row r="4" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
-      <c r="C4" s="3">
+      <c r="B4" s="14">
         <v>0</v>
       </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="10"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
+      <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="10"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="3"/>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="9"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3">
+      <c r="R4" s="3">
         <v>2</v>
       </c>
+      <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="10"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3">
+      <c r="W4" s="3">
         <v>3</v>
       </c>
+      <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="10"/>
       <c r="AA4" s="9"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3">
+      <c r="AB4" s="3">
         <v>4</v>
       </c>
+      <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="17"/>
     </row>
@@ -2278,44 +2385,44 @@
       </c>
     </row>
     <row r="7" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="3">
+      <c r="B7" s="14">
         <v>5</v>
       </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="10"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="3">
-        <v>6</v>
-      </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="10"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="3"/>
+      <c r="M7" s="3">
+        <v>6</v>
+      </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="9"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3">
+      <c r="R7" s="3">
         <v>7</v>
       </c>
+      <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="10"/>
       <c r="V7" s="9"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3">
+      <c r="W7" s="3">
         <v>8</v>
       </c>
+      <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="10"/>
       <c r="AA7" s="9"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3">
+      <c r="AB7" s="3">
         <v>9</v>
       </c>
+      <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
       <c r="AE7" s="17"/>
     </row>
@@ -2505,16 +2612,12 @@
     </row>
     <row r="10" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
-      <c r="C10" s="3">
-        <v>10</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="10"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="3">
-        <v>11</v>
-      </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="10"/>
@@ -2525,23 +2628,17 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="3">
-        <v>12</v>
-      </c>
+      <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="10"/>
       <c r="V10" s="9"/>
       <c r="W10" s="3"/>
-      <c r="X10" s="3">
-        <v>13</v>
-      </c>
+      <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="10"/>
       <c r="AA10" s="9"/>
       <c r="AB10" s="3"/>
-      <c r="AC10" s="3">
-        <v>14</v>
-      </c>
+      <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="17"/>
     </row>
@@ -2731,12 +2828,16 @@
     </row>
     <row r="13" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3">
+        <v>10</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="10"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3">
+        <v>11</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="10"/>
@@ -2747,17 +2848,23 @@
       <c r="P13" s="10"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
+      <c r="S13" s="3">
+        <v>12</v>
+      </c>
       <c r="T13" s="3"/>
       <c r="U13" s="10"/>
       <c r="V13" s="9"/>
       <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
+      <c r="X13" s="3">
+        <v>13</v>
+      </c>
       <c r="Y13" s="3"/>
       <c r="Z13" s="10"/>
       <c r="AA13" s="9"/>
       <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
+      <c r="AC13" s="3">
+        <v>14</v>
+      </c>
       <c r="AD13" s="3"/>
       <c r="AE13" s="17"/>
     </row>
@@ -2947,44 +3054,44 @@
     </row>
     <row r="16" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="14"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3">
+      <c r="C16" s="3">
         <v>15</v>
       </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="10"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3">
+      <c r="H16" s="3">
         <v>16</v>
       </c>
+      <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="10"/>
       <c r="L16" s="9"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="3">
-        <v>17</v>
-      </c>
+      <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
+      <c r="S16" s="3">
+        <v>17</v>
+      </c>
       <c r="T16" s="3"/>
       <c r="U16" s="10"/>
       <c r="V16" s="9"/>
       <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3">
+      <c r="X16" s="3">
         <v>18</v>
       </c>
+      <c r="Y16" s="3"/>
       <c r="Z16" s="10"/>
       <c r="AA16" s="9"/>
       <c r="AB16" s="3"/>
-      <c r="AC16" s="3"/>
-      <c r="AD16" s="3">
+      <c r="AC16" s="3">
         <v>19</v>
       </c>
+      <c r="AD16" s="3"/>
       <c r="AE16" s="17"/>
     </row>
     <row r="17" spans="2:31" x14ac:dyDescent="0.25">
@@ -3173,44 +3280,44 @@
     </row>
     <row r="19" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="14"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3">
+      <c r="C19" s="3">
         <v>20</v>
       </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="10"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3">
+      <c r="H19" s="3">
         <v>21</v>
       </c>
+      <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="10"/>
       <c r="L19" s="9"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="3">
-        <v>22</v>
-      </c>
+      <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="10"/>
       <c r="Q19" s="9"/>
       <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="S19" s="3">
+        <v>22</v>
+      </c>
       <c r="T19" s="3"/>
       <c r="U19" s="10"/>
       <c r="V19" s="9"/>
       <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3">
+      <c r="X19" s="3">
         <v>23</v>
       </c>
+      <c r="Y19" s="3"/>
       <c r="Z19" s="10"/>
       <c r="AA19" s="9"/>
       <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3">
+      <c r="AC19" s="3">
         <v>24</v>
       </c>
+      <c r="AD19" s="3"/>
       <c r="AE19" s="17"/>
     </row>
     <row r="20" spans="2:31" x14ac:dyDescent="0.25">
@@ -3399,44 +3506,44 @@
     </row>
     <row r="22" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="14"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3">
+      <c r="C22" s="3">
         <v>25</v>
       </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="10"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3">
+      <c r="H22" s="3">
         <v>26</v>
       </c>
+      <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="10"/>
       <c r="L22" s="9"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="3">
-        <v>27</v>
-      </c>
+      <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="10"/>
       <c r="Q22" s="9"/>
       <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
+      <c r="S22" s="3">
+        <v>27</v>
+      </c>
       <c r="T22" s="3"/>
       <c r="U22" s="10"/>
       <c r="V22" s="9"/>
       <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3">
+      <c r="X22" s="3">
         <v>28</v>
       </c>
+      <c r="Y22" s="3"/>
       <c r="Z22" s="10"/>
       <c r="AA22" s="9"/>
       <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3">
+      <c r="AC22" s="3">
         <v>29</v>
       </c>
+      <c r="AD22" s="3"/>
       <c r="AE22" s="17"/>
     </row>
     <row r="24" spans="2:31" x14ac:dyDescent="0.25">
@@ -3444,12 +3551,7 @@
         <v>210</v>
       </c>
       <c r="J24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="U25">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:31" x14ac:dyDescent="0.25">
@@ -3457,33 +3559,79 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <f>B26/5</f>
+        <f>(B26/30)*6</f>
         <v>0</v>
       </c>
       <c r="G26">
         <f>ROUNDDOWN(F26,0)</f>
         <v>0</v>
       </c>
+      <c r="H26">
+        <f>30*G26</f>
+        <v>0</v>
+      </c>
       <c r="I26">
-        <f>$B26*5+$J$24-1</f>
-        <v>2</v>
-      </c>
-      <c r="J26">
-        <f>$B26*5+$J$24-2</f>
-        <v>1</v>
+        <f>(G26+1)*30</f>
+        <v>30</v>
       </c>
       <c r="K26">
-        <f>(($B26+1)*5)+$J$24</f>
-        <v>8</v>
-      </c>
-      <c r="M26" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="U26" s="21" t="s">
-        <v>213</v>
+        <f>B26-(G26*5)</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>(K26/5)*5</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>L26*5</f>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f>(L26+1)*5</f>
+        <v>5</v>
+      </c>
+      <c r="O26">
+        <f>I26+M26</f>
+        <v>30</v>
+      </c>
+      <c r="P26">
+        <f>I26+N26</f>
+        <v>35</v>
+      </c>
+      <c r="R26">
+        <f>H26+M26</f>
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <f>I26+M26</f>
+        <v>30</v>
+      </c>
+      <c r="T26">
+        <f>H26+N26</f>
+        <v>5</v>
+      </c>
+      <c r="U26">
+        <f>I26+N26</f>
+        <v>35</v>
+      </c>
+      <c r="W26">
+        <f>R26-C26</f>
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <f>S26-C26</f>
+        <v>30</v>
+      </c>
+      <c r="Y26">
+        <f>T26-C26</f>
+        <v>5</v>
+      </c>
+      <c r="Z26">
+        <f>U26-C26</f>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:31" x14ac:dyDescent="0.25">
@@ -3491,31 +3639,83 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D27">
         <f>C27-C26</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27:F49" si="0">B27/5</f>
+        <f t="shared" ref="F27:F55" si="0">(B27/30)*6</f>
         <v>0.2</v>
       </c>
       <c r="G27">
         <f t="shared" ref="G27:G55" si="1">ROUNDDOWN(F27,0)</f>
         <v>0</v>
       </c>
+      <c r="H27">
+        <f t="shared" ref="H27:H55" si="2">30*G27</f>
+        <v>0</v>
+      </c>
       <c r="I27">
-        <f t="shared" ref="I27:I55" si="2">$B27*5+$J$24-1</f>
-        <v>7</v>
-      </c>
-      <c r="J27">
-        <f t="shared" ref="J27:J55" si="3">$B27*5+$J$24-2</f>
-        <v>6</v>
+        <f t="shared" ref="I27:I55" si="3">(G27+1)*30</f>
+        <v>30</v>
       </c>
       <c r="K27">
-        <f t="shared" ref="K27:K55" si="4">(($B27+1)*5)+$J$24</f>
-        <v>13</v>
+        <f t="shared" ref="K27:K55" si="4">B27-(G27*5)</f>
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <f t="shared" ref="L27:L55" si="5">(K27/5)*5</f>
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:M55" si="6">L27*5</f>
+        <v>5</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ref="N27:N55" si="7">(L27+1)*5</f>
+        <v>10</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ref="O27:O55" si="8">I27+M27</f>
+        <v>35</v>
+      </c>
+      <c r="P27">
+        <f t="shared" ref="P27:P55" si="9">I27+N27</f>
+        <v>40</v>
+      </c>
+      <c r="R27">
+        <f t="shared" ref="R27:R55" si="10">H27+M27</f>
+        <v>5</v>
+      </c>
+      <c r="S27">
+        <f t="shared" ref="S27:S55" si="11">I27+M27</f>
+        <v>35</v>
+      </c>
+      <c r="T27">
+        <f t="shared" ref="T27:T55" si="12">H27+N27</f>
+        <v>10</v>
+      </c>
+      <c r="U27">
+        <f t="shared" ref="U27:U55" si="13">I27+N27</f>
+        <v>40</v>
+      </c>
+      <c r="W27">
+        <f t="shared" ref="W27:W55" si="14">R27-C27</f>
+        <v>-6</v>
+      </c>
+      <c r="X27">
+        <f t="shared" ref="X27:X55" si="15">S27-C27</f>
+        <v>24</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" ref="Y27:Y55" si="16">T27-C27</f>
+        <v>-1</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" ref="Z27:Z55" si="17">U27-C27</f>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:31" x14ac:dyDescent="0.25">
@@ -3523,11 +3723,11 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:D55" si="5">C28-C27</f>
-        <v>11</v>
+        <f t="shared" ref="D28:D55" si="18">C28-C27</f>
+        <v>5</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
@@ -3537,23 +3737,69 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="I28">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="J28">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="K28">
         <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="M28" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="U28" s="21" t="s">
-        <v>215</v>
+        <v>2</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="9"/>
+        <v>45</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="14"/>
+        <v>-6</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="17"/>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:31" x14ac:dyDescent="0.25">
@@ -3561,31 +3807,83 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="I29">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="J29">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="K29">
         <f t="shared" si="4"/>
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="13"/>
+        <v>50</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="14"/>
+        <v>-6</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="17"/>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="2:31" x14ac:dyDescent="0.25">
@@ -3593,10 +3891,10 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F30">
@@ -3607,17 +3905,69 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="I30">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="J30">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K30">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="9"/>
+        <v>55</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="11"/>
+        <v>50</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="12"/>
+        <v>25</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="13"/>
+        <v>55</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="14"/>
+        <v>-6</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="17"/>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="2:31" x14ac:dyDescent="0.25">
@@ -3625,10 +3975,10 @@
         <v>5</v>
       </c>
       <c r="C31">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="F31">
@@ -3639,17 +3989,69 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
       <c r="I31">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="J31">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="K31">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="9"/>
+        <v>65</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="12"/>
+        <v>35</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="13"/>
+        <v>65</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="17"/>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="2:31" x14ac:dyDescent="0.25">
@@ -3657,43 +4059,95 @@
         <v>6</v>
       </c>
       <c r="C32">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D32">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="18"/>
+        <v>11</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
       <c r="I32">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="J32">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="K32">
         <f t="shared" si="4"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="9"/>
+        <v>70</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="10"/>
+        <v>35</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="11"/>
+        <v>65</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="13"/>
+        <v>70</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="14"/>
+        <v>-6</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="17"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>7</v>
       </c>
       <c r="C33">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D33">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
@@ -3703,28 +4157,80 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
       <c r="I33">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="J33">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="K33">
         <f t="shared" si="4"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="9"/>
+        <v>75</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="11"/>
+        <v>70</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="12"/>
+        <v>45</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="14"/>
+        <v>-6</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="17"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>8</v>
       </c>
       <c r="C34">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F34">
@@ -3735,156 +4241,424 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
       <c r="I34">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="J34">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="K34">
         <f t="shared" si="4"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="12"/>
+        <v>50</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="13"/>
+        <v>80</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="14"/>
+        <v>-6</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="17"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B35" s="22">
         <v>9</v>
       </c>
-      <c r="C35">
-        <v>57</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="5"/>
+      <c r="C35" s="22">
+        <v>56</v>
+      </c>
+      <c r="D35" s="22">
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="F35">
+      <c r="E35" s="22"/>
+      <c r="F35" s="22">
         <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="G35">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="G35" s="22">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I35">
+      <c r="H35" s="22">
         <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="J35">
+        <v>30</v>
+      </c>
+      <c r="I35" s="22">
         <f t="shared" si="3"/>
-        <v>46</v>
-      </c>
-      <c r="K35">
+        <v>60</v>
+      </c>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22">
         <f t="shared" si="4"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <v>10</v>
-      </c>
-      <c r="C36">
-        <v>61</v>
-      </c>
-      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="L35" s="22">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="F36">
+      <c r="M35" s="22">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="N35" s="22">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="O35" s="22">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="P35" s="22">
+        <f t="shared" si="9"/>
+        <v>85</v>
+      </c>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22">
+        <f t="shared" si="10"/>
+        <v>50</v>
+      </c>
+      <c r="S35" s="22">
+        <f t="shared" si="11"/>
+        <v>80</v>
+      </c>
+      <c r="T35" s="22">
+        <f t="shared" si="12"/>
+        <v>55</v>
+      </c>
+      <c r="U35" s="22">
+        <f t="shared" si="13"/>
+        <v>85</v>
+      </c>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22">
+        <f t="shared" si="14"/>
+        <v>-6</v>
+      </c>
+      <c r="X35" s="22">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="Y35" s="22">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="Z35" s="22">
+        <f t="shared" si="17"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B36" s="23">
+        <v>10</v>
+      </c>
+      <c r="C36" s="23">
+        <v>91</v>
+      </c>
+      <c r="D36" s="23">
+        <f t="shared" si="18"/>
+        <v>35</v>
+      </c>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="23">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I36">
+      <c r="H36" s="23">
         <f t="shared" si="2"/>
-        <v>52</v>
-      </c>
-      <c r="J36">
+        <v>60</v>
+      </c>
+      <c r="I36" s="23">
         <f t="shared" si="3"/>
-        <v>51</v>
-      </c>
-      <c r="K36">
+        <v>90</v>
+      </c>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23">
         <f t="shared" si="4"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="L36" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="23">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="O36" s="23">
+        <f t="shared" si="8"/>
+        <v>90</v>
+      </c>
+      <c r="P36" s="23">
+        <f t="shared" si="9"/>
+        <v>95</v>
+      </c>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23">
+        <f t="shared" si="10"/>
+        <v>60</v>
+      </c>
+      <c r="S36" s="23">
+        <f t="shared" si="11"/>
+        <v>90</v>
+      </c>
+      <c r="T36" s="23">
+        <f t="shared" si="12"/>
+        <v>65</v>
+      </c>
+      <c r="U36" s="23">
+        <f t="shared" si="13"/>
+        <v>95</v>
+      </c>
+      <c r="V36" s="23"/>
+      <c r="W36" s="23">
+        <f t="shared" si="14"/>
+        <v>-31</v>
+      </c>
+      <c r="X36" s="23">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="Y36" s="23">
+        <f t="shared" si="16"/>
+        <v>-26</v>
+      </c>
+      <c r="Z36" s="23">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>11</v>
       </c>
       <c r="C37">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="D37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>2.1999999999999997</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
       <c r="I37">
-        <f t="shared" si="2"/>
-        <v>57</v>
-      </c>
-      <c r="J37">
         <f t="shared" si="3"/>
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="K37">
         <f t="shared" si="4"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="8"/>
+        <v>95</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="10"/>
+        <v>65</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="11"/>
+        <v>95</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="14"/>
+        <v>-31</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="16"/>
+        <v>-26</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>12</v>
       </c>
       <c r="C38">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="D38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>2.4</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
       <c r="I38">
-        <f t="shared" si="2"/>
-        <v>62</v>
-      </c>
-      <c r="J38">
         <f t="shared" si="3"/>
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="K38">
         <f t="shared" si="4"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="9"/>
+        <v>105</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="10"/>
+        <v>70</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="13"/>
+        <v>105</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>13</v>
       </c>
       <c r="C39">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="D39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F39">
@@ -3895,28 +4669,80 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
       <c r="I39">
-        <f t="shared" si="2"/>
-        <v>67</v>
-      </c>
-      <c r="J39">
         <f t="shared" si="3"/>
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="K39">
         <f t="shared" si="4"/>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="8"/>
+        <v>105</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="9"/>
+        <v>110</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="10"/>
+        <v>75</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="11"/>
+        <v>105</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="12"/>
+        <v>80</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="13"/>
+        <v>110</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>14</v>
       </c>
       <c r="C40">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="D40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F40">
@@ -3927,29 +4753,81 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="H40">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
       <c r="I40">
-        <f t="shared" si="2"/>
-        <v>72</v>
-      </c>
-      <c r="J40">
         <f t="shared" si="3"/>
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="K40">
         <f t="shared" si="4"/>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="8"/>
+        <v>110</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="9"/>
+        <v>115</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="10"/>
+        <v>80</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="11"/>
+        <v>110</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="12"/>
+        <v>85</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="13"/>
+        <v>115</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>15</v>
       </c>
       <c r="C41">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D41">
-        <f t="shared" si="5"/>
-        <v>35</v>
+        <f t="shared" si="18"/>
+        <v>4</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
@@ -3959,28 +4837,80 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="H41">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
       <c r="I41">
-        <f t="shared" si="2"/>
-        <v>77</v>
-      </c>
-      <c r="J41">
         <f t="shared" si="3"/>
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="K41">
         <f t="shared" si="4"/>
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="8"/>
+        <v>120</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="9"/>
+        <v>125</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="10"/>
+        <v>90</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="11"/>
+        <v>120</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="12"/>
+        <v>95</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="13"/>
+        <v>125</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="14"/>
+        <v>-31</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="16"/>
+        <v>-26</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>16</v>
       </c>
       <c r="C42">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F42">
@@ -3991,29 +4921,81 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="H42">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
       <c r="I42">
-        <f t="shared" si="2"/>
-        <v>82</v>
-      </c>
-      <c r="J42">
         <f t="shared" si="3"/>
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="K42">
         <f t="shared" si="4"/>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="8"/>
+        <v>125</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="9"/>
+        <v>130</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="10"/>
+        <v>95</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="11"/>
+        <v>125</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="12"/>
+        <v>100</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="13"/>
+        <v>130</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="14"/>
+        <v>-31</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="16"/>
+        <v>-26</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>17</v>
       </c>
       <c r="C43">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D43">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="18"/>
+        <v>11</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
@@ -4023,60 +5005,164 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="H43">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
       <c r="I43">
-        <f t="shared" si="2"/>
-        <v>87</v>
-      </c>
-      <c r="J43">
         <f t="shared" si="3"/>
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="K43">
         <f t="shared" si="4"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="8"/>
+        <v>130</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="9"/>
+        <v>135</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="11"/>
+        <v>130</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="12"/>
+        <v>105</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="13"/>
+        <v>135</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z43">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>18</v>
       </c>
       <c r="C44">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D44">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
-        <v>3.6</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="G44">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="H44">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
       <c r="I44">
-        <f t="shared" si="2"/>
-        <v>92</v>
-      </c>
-      <c r="J44">
         <f t="shared" si="3"/>
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="K44">
         <f t="shared" si="4"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="8"/>
+        <v>135</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="9"/>
+        <v>140</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="10"/>
+        <v>105</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="11"/>
+        <v>135</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="12"/>
+        <v>110</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="13"/>
+        <v>140</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z44">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>19</v>
       </c>
       <c r="C45">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F45">
@@ -4087,28 +5173,80 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="H45">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
       <c r="I45">
-        <f t="shared" si="2"/>
-        <v>97</v>
-      </c>
-      <c r="J45">
         <f t="shared" si="3"/>
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="K45">
         <f t="shared" si="4"/>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="8"/>
+        <v>140</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="9"/>
+        <v>145</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="10"/>
+        <v>110</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="11"/>
+        <v>140</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="12"/>
+        <v>115</v>
+      </c>
+      <c r="U45">
+        <f t="shared" si="13"/>
+        <v>145</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X45">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y45">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z45">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>20</v>
       </c>
       <c r="C46">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="F46">
@@ -4119,305 +5257,846 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="H46">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
       <c r="I46">
-        <f t="shared" si="2"/>
-        <v>102</v>
-      </c>
-      <c r="J46">
         <f t="shared" si="3"/>
-        <v>101</v>
+        <v>150</v>
       </c>
       <c r="K46">
         <f t="shared" si="4"/>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="8"/>
+        <v>150</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="9"/>
+        <v>155</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="10"/>
+        <v>120</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="11"/>
+        <v>150</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="12"/>
+        <v>125</v>
+      </c>
+      <c r="U46">
+        <f t="shared" si="13"/>
+        <v>155</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="14"/>
+        <v>-31</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" si="16"/>
+        <v>-26</v>
+      </c>
+      <c r="Z46">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>21</v>
       </c>
       <c r="C47">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>4.1999999999999993</v>
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="H47">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
       <c r="I47">
-        <f t="shared" si="2"/>
-        <v>107</v>
-      </c>
-      <c r="J47">
         <f t="shared" si="3"/>
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="K47">
         <f t="shared" si="4"/>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="8"/>
+        <v>155</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="9"/>
+        <v>160</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="10"/>
+        <v>125</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="11"/>
+        <v>155</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="12"/>
+        <v>130</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="13"/>
+        <v>160</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="14"/>
+        <v>-31</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="Y47">
+        <f t="shared" si="16"/>
+        <v>-26</v>
+      </c>
+      <c r="Z47">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>22</v>
       </c>
       <c r="C48">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D48">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="18"/>
+        <v>11</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>4.3999999999999995</v>
       </c>
       <c r="G48">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="H48">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
       <c r="I48">
-        <f t="shared" si="2"/>
-        <v>112</v>
-      </c>
-      <c r="J48">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="K48">
         <f t="shared" si="4"/>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="8"/>
+        <v>160</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="9"/>
+        <v>165</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="10"/>
+        <v>130</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="11"/>
+        <v>160</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="12"/>
+        <v>135</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="13"/>
+        <v>165</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y48">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z48">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>23</v>
       </c>
       <c r="C49">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D49">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="G49">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="H49">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
       <c r="I49">
-        <f t="shared" si="2"/>
-        <v>117</v>
-      </c>
-      <c r="J49">
         <f t="shared" si="3"/>
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="K49">
         <f t="shared" si="4"/>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="8"/>
+        <v>165</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="9"/>
+        <v>170</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="10"/>
+        <v>135</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="11"/>
+        <v>165</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="12"/>
+        <v>140</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="13"/>
+        <v>170</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>24</v>
       </c>
       <c r="C50">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F50">
-        <f t="shared" ref="F50:F55" si="6">B50/5</f>
-        <v>4.8</v>
+        <f t="shared" si="0"/>
+        <v>4.8000000000000007</v>
       </c>
       <c r="G50">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="H50">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
       <c r="I50">
-        <f t="shared" si="2"/>
-        <v>122</v>
-      </c>
-      <c r="J50">
         <f t="shared" si="3"/>
-        <v>121</v>
+        <v>150</v>
       </c>
       <c r="K50">
         <f t="shared" si="4"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="8"/>
+        <v>170</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="9"/>
+        <v>175</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="10"/>
+        <v>140</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="11"/>
+        <v>170</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="12"/>
+        <v>145</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="13"/>
+        <v>175</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X50">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y50">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z50">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>25</v>
       </c>
       <c r="C51">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="F51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G51">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="H51">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
       <c r="I51">
-        <f t="shared" si="2"/>
-        <v>127</v>
-      </c>
-      <c r="J51">
         <f t="shared" si="3"/>
-        <v>126</v>
+        <v>180</v>
       </c>
       <c r="K51">
         <f t="shared" si="4"/>
-        <v>133</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="8"/>
+        <v>180</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="9"/>
+        <v>185</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="10"/>
+        <v>150</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="11"/>
+        <v>180</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="12"/>
+        <v>155</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="13"/>
+        <v>185</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="14"/>
+        <v>-31</v>
+      </c>
+      <c r="X51">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="Y51">
+        <f t="shared" si="16"/>
+        <v>-26</v>
+      </c>
+      <c r="Z51">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>26</v>
       </c>
       <c r="C52">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>5.2</v>
       </c>
       <c r="G52">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="H52">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
       <c r="I52">
-        <f t="shared" si="2"/>
-        <v>132</v>
-      </c>
-      <c r="J52">
         <f t="shared" si="3"/>
-        <v>131</v>
+        <v>180</v>
       </c>
       <c r="K52">
         <f t="shared" si="4"/>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="8"/>
+        <v>185</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="9"/>
+        <v>190</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="10"/>
+        <v>155</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="11"/>
+        <v>185</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="12"/>
+        <v>160</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="13"/>
+        <v>190</v>
+      </c>
+      <c r="W52">
+        <f t="shared" si="14"/>
+        <v>-31</v>
+      </c>
+      <c r="X52">
+        <f t="shared" si="15"/>
+        <v>-1</v>
+      </c>
+      <c r="Y52">
+        <f t="shared" si="16"/>
+        <v>-26</v>
+      </c>
+      <c r="Z52">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>27</v>
       </c>
       <c r="C53">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D53">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="18"/>
+        <v>11</v>
       </c>
       <c r="F53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
       <c r="G53">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="H53">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
       <c r="I53">
-        <f t="shared" si="2"/>
-        <v>137</v>
-      </c>
-      <c r="J53">
         <f t="shared" si="3"/>
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="K53">
         <f t="shared" si="4"/>
-        <v>143</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="8"/>
+        <v>190</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="9"/>
+        <v>195</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="10"/>
+        <v>160</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="11"/>
+        <v>190</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="12"/>
+        <v>165</v>
+      </c>
+      <c r="U53">
+        <f t="shared" si="13"/>
+        <v>195</v>
+      </c>
+      <c r="W53">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X53">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y53">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z53">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>28</v>
       </c>
       <c r="C54">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D54">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
       <c r="F54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="G54">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="H54">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
       <c r="I54">
-        <f t="shared" si="2"/>
-        <v>142</v>
-      </c>
-      <c r="J54">
         <f t="shared" si="3"/>
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="K54">
         <f t="shared" si="4"/>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="8"/>
+        <v>195</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="9"/>
+        <v>200</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="10"/>
+        <v>165</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="11"/>
+        <v>195</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="12"/>
+        <v>170</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="13"/>
+        <v>200</v>
+      </c>
+      <c r="W54">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X54">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y54">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z54">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>29</v>
       </c>
       <c r="C55">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>5.8</v>
       </c>
       <c r="G55">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="H55">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
       <c r="I55">
-        <f t="shared" si="2"/>
-        <v>147</v>
-      </c>
-      <c r="J55">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="K55">
         <f t="shared" si="4"/>
-        <v>153</v>
+        <v>4</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="8"/>
+        <v>200</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="9"/>
+        <v>205</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="10"/>
+        <v>170</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="11"/>
+        <v>200</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="12"/>
+        <v>175</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="13"/>
+        <v>205</v>
+      </c>
+      <c r="W55">
+        <f t="shared" si="14"/>
+        <v>-37</v>
+      </c>
+      <c r="X55">
+        <f t="shared" si="15"/>
+        <v>-7</v>
+      </c>
+      <c r="Y55">
+        <f t="shared" si="16"/>
+        <v>-32</v>
+      </c>
+      <c r="Z55">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B58" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="60" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B60" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued with the message composition.  Not much progress so far.
</commit_message>
<xml_diff>
--- a/7 node grid.xlsx
+++ b/7 node grid.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Round 1" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="227">
   <si>
     <t>1.2.3</t>
   </si>
@@ -698,6 +698,18 @@
   </si>
   <si>
     <t>gen</t>
+  </si>
+  <si>
+    <t>sen 1</t>
+  </si>
+  <si>
+    <t>sen 2</t>
+  </si>
+  <si>
+    <t>sen 5</t>
+  </si>
+  <si>
+    <t>sen 7</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -1466,7 +1478,7 @@
   <dimension ref="B1:R46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6795,23 +6807,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F22"/>
+  <dimension ref="B1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E8"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="18">
         <v>1</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="21" t="s">
+        <v>223</v>
+      </c>
       <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="19">
         <v>0</v>
       </c>
@@ -6819,20 +6842,56 @@
         <v>0</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="18">
         <v>2</v>
       </c>
@@ -6840,10 +6899,28 @@
         <v>2</v>
       </c>
       <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="19">
         <v>1</v>
       </c>
@@ -6851,19 +6928,55 @@
         <v>3</v>
       </c>
       <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="G6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="20"/>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="G7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="18">
         <v>3</v>
       </c>
@@ -6871,41 +6984,59 @@
         <v>5</v>
       </c>
       <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="G8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="20"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="20"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="19">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="20"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -6941,15 +7072,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O31"/>
+  <dimension ref="B1:O65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N1" t="s">
+        <v>224</v>
+      </c>
+    </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="12">
         <v>1.2</v>
@@ -7733,6 +7871,28 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>B24/5</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>ROUNDDOWN(C24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>D24*6</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f>(D24+1)*6</f>
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
       <c r="I24">
         <v>22</v>
       </c>
@@ -7755,6 +7915,28 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C65" si="2">B25/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:D65" si="3">ROUNDDOWN(C25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ref="E25:E65" si="4">D25*6</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25:F65" si="5">(D25+1)*6</f>
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
       <c r="I25">
         <v>23</v>
       </c>
@@ -7777,6 +7959,28 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
       <c r="I26">
         <v>24</v>
       </c>
@@ -7799,6 +8003,28 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
       <c r="I27">
         <v>25</v>
       </c>
@@ -7821,6 +8047,28 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
       <c r="I28">
         <v>26</v>
       </c>
@@ -7843,6 +8091,28 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G29">
+        <v>12</v>
+      </c>
       <c r="I29">
         <v>27</v>
       </c>
@@ -7865,6 +8135,28 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G30">
+        <v>14</v>
+      </c>
       <c r="I30">
         <v>28</v>
       </c>
@@ -7887,6 +8179,28 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G31">
+        <v>15</v>
+      </c>
       <c r="I31">
         <v>29</v>
       </c>
@@ -7906,6 +8220,786 @@
       <c r="O31">
         <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>1.8</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="G34">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="G35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>2.4</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="G36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>2.6</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="G37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>2.8</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="G38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="G39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>16</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>3.2</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="G40">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>3.4</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="G41">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>18</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>3.6</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="G42">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>19</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>3.8</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="G43">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="G44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>21</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>4.2</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="G45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>22</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="G46">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>23</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="G47">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>24</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>4.8</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="G48">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>25</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="G49">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>26</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>5.2</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="G50">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>27</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>5.4</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="G51">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>28</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>5.6</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="G52">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>29</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>5.8</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="G53">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>30</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>31</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>6.2</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>32</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="2"/>
+        <v>6.4</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>33</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="2"/>
+        <v>6.6</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>34</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="2"/>
+        <v>6.8</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>35</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>36</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="2"/>
+        <v>7.2</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>37</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="2"/>
+        <v>7.4</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>38</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="2"/>
+        <v>7.6</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>39</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="2"/>
+        <v>7.8</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>40</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>41</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="2"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="5"/>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -7917,7 +9011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AE60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished the step messages, started on the bottom up messages.
</commit_message>
<xml_diff>
--- a/7 node grid.xlsx
+++ b/7 node grid.xlsx
@@ -6810,7 +6810,7 @@
   <dimension ref="B1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7074,8 +7074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7891,7 +7891,11 @@
         <v>6</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <f>B24-(D24*(6-1))</f>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>22</v>
@@ -7935,7 +7939,11 @@
         <v>6</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H53" si="6">B25-(D25*(6-1))</f>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>23</v>
@@ -7979,7 +7987,11 @@
         <v>6</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
       <c r="I26">
         <v>24</v>
@@ -8023,7 +8035,11 @@
         <v>6</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="I27">
         <v>25</v>
@@ -8067,7 +8083,11 @@
         <v>6</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="I28">
         <v>26</v>
@@ -8111,7 +8131,11 @@
         <v>12</v>
       </c>
       <c r="G29">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="I29">
         <v>27</v>
@@ -8157,6 +8181,10 @@
       <c r="G30">
         <v>14</v>
       </c>
+      <c r="H30">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
       <c r="I30">
         <v>28</v>
       </c>
@@ -8201,6 +8229,10 @@
       <c r="G31">
         <v>15</v>
       </c>
+      <c r="H31">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
       <c r="I31">
         <v>29</v>
       </c>
@@ -8245,8 +8277,12 @@
       <c r="G32">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>9</v>
       </c>
@@ -8269,8 +8305,12 @@
       <c r="G33">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>10</v>
       </c>
@@ -8291,10 +8331,14 @@
         <v>18</v>
       </c>
       <c r="G34">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>11</v>
       </c>
@@ -8317,8 +8361,12 @@
       <c r="G35">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>12</v>
       </c>
@@ -8341,8 +8389,12 @@
       <c r="G36">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>13</v>
       </c>
@@ -8365,8 +8417,12 @@
       <c r="G37">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>14</v>
       </c>
@@ -8389,8 +8445,12 @@
       <c r="G38">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>15</v>
       </c>
@@ -8411,10 +8471,14 @@
         <v>24</v>
       </c>
       <c r="G39">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>16</v>
       </c>
@@ -8437,8 +8501,12 @@
       <c r="G40">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>17</v>
       </c>
@@ -8461,8 +8529,12 @@
       <c r="G41">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>18</v>
       </c>
@@ -8485,8 +8557,12 @@
       <c r="G42">
         <v>28</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>19</v>
       </c>
@@ -8509,8 +8585,12 @@
       <c r="G43">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>20</v>
       </c>
@@ -8531,10 +8611,14 @@
         <v>30</v>
       </c>
       <c r="G44">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>21</v>
       </c>
@@ -8555,10 +8639,14 @@
         <v>30</v>
       </c>
       <c r="G45">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>22</v>
       </c>
@@ -8581,8 +8669,12 @@
       <c r="G46">
         <v>33</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>23</v>
       </c>
@@ -8605,8 +8697,12 @@
       <c r="G47">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>24</v>
       </c>
@@ -8629,8 +8725,12 @@
       <c r="G48">
         <v>35</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>25</v>
       </c>
@@ -8651,10 +8751,14 @@
         <v>36</v>
       </c>
       <c r="G49">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>26</v>
       </c>
@@ -8677,8 +8781,12 @@
       <c r="G50">
         <v>38</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>27</v>
       </c>
@@ -8701,8 +8809,12 @@
       <c r="G51">
         <v>39</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>28</v>
       </c>
@@ -8725,8 +8837,12 @@
       <c r="G52">
         <v>40</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>29</v>
       </c>
@@ -8749,8 +8865,12 @@
       <c r="G53">
         <v>41</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>30</v>
       </c>
@@ -8771,7 +8891,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>31</v>
       </c>
@@ -8792,7 +8912,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>32</v>
       </c>
@@ -8813,7 +8933,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>33</v>
       </c>
@@ -8834,7 +8954,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>34</v>
       </c>
@@ -8855,7 +8975,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>35</v>
       </c>
@@ -8876,7 +8996,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>36</v>
       </c>
@@ -8897,7 +9017,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>37</v>
       </c>
@@ -8918,7 +9038,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>38</v>
       </c>
@@ -8939,7 +9059,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>39</v>
       </c>
@@ -8960,7 +9080,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>40</v>
       </c>

</xml_diff>